<commit_message>
new file:   Indecate_energy.html 	modified:   Indecate_energy.py 	deleted:    New Text Document.html 	new file:   data/Results_Scenarios_TESTING - oldCopy.xlsx 	modified:   data/Results_Scenarios_TESTING.xlsx 	new file:   energy_breakdown_glass.csv
</commit_message>
<xml_diff>
--- a/data/Results_Scenarios_TESTING.xlsx
+++ b/data/Results_Scenarios_TESTING.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msalman\Desktop\OSMOSE ETs\Python work\INDECATE2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1A00AE-ECB2-4CFA-AE79-67503D7B577B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F66E14-507D-4A74-B83C-8D9F4A14EA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="710" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="710" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NG" sheetId="1" r:id="rId1"/>
@@ -31,11 +31,46 @@
     <sheet name="energy breakdown" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="82">
   <si>
     <t>Lines</t>
   </si>
@@ -279,12 +314,15 @@
   <si>
     <t>Qel-WHR</t>
   </si>
+  <si>
+    <t>THESE ARE JGDs SUMS: CAUTION</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,16 +340,322 @@
       <sz val="11"/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -389,11 +733,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -406,9 +898,57 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1 2" xfId="19" xr:uid="{AF3AF8AA-8C34-42A1-9881-A95A717F4AB6}"/>
+    <cellStyle name="20% - Accent2 2" xfId="23" xr:uid="{023CE91F-04E3-4B3F-A7BB-81E92EA92065}"/>
+    <cellStyle name="20% - Accent3 2" xfId="27" xr:uid="{AF4C5158-1F0C-4258-AA13-24BDCE65228F}"/>
+    <cellStyle name="20% - Accent4 2" xfId="31" xr:uid="{FE3733F8-207F-4C38-99AE-6548331314CC}"/>
+    <cellStyle name="20% - Accent5 2" xfId="35" xr:uid="{9A1FBACF-85F1-451B-A4EA-258EB7038C6A}"/>
+    <cellStyle name="20% - Accent6 2" xfId="39" xr:uid="{258170BD-AB61-4889-BF1B-EDE07C6D0034}"/>
+    <cellStyle name="40% - Accent1 2" xfId="20" xr:uid="{95FF68D5-7292-47F2-AF52-ED542EA34EEA}"/>
+    <cellStyle name="40% - Accent2 2" xfId="24" xr:uid="{63D965C9-3647-4BF6-AA09-B7E2BCB2E8F8}"/>
+    <cellStyle name="40% - Accent3 2" xfId="28" xr:uid="{593B2FFB-15E5-4168-A3A1-4F0EB6D533DC}"/>
+    <cellStyle name="40% - Accent4 2" xfId="32" xr:uid="{787E9DA9-483E-46C4-AE32-5101D17684C8}"/>
+    <cellStyle name="40% - Accent5 2" xfId="36" xr:uid="{8B6EF97A-05A9-47A5-B538-7C829354CBA7}"/>
+    <cellStyle name="40% - Accent6 2" xfId="40" xr:uid="{538BE4C3-C5C2-4DDA-BE43-D4D0D20939C8}"/>
+    <cellStyle name="60% - Accent1 2" xfId="21" xr:uid="{BF9A6167-C1B6-4DF1-B07E-423ABBA3DC71}"/>
+    <cellStyle name="60% - Accent2 2" xfId="25" xr:uid="{22C3BF4F-4984-4078-83FC-4CFB706F3A1E}"/>
+    <cellStyle name="60% - Accent3 2" xfId="29" xr:uid="{393395A6-D744-4A87-BBF1-00595EFFA99B}"/>
+    <cellStyle name="60% - Accent4 2" xfId="33" xr:uid="{2AED6982-B574-48E1-AFC6-B8333F2EC242}"/>
+    <cellStyle name="60% - Accent5 2" xfId="37" xr:uid="{5FC7411F-027F-45FC-9081-13855CF4275D}"/>
+    <cellStyle name="60% - Accent6 2" xfId="41" xr:uid="{8FBAA8A2-5B5F-4105-88B8-AB4809BB24A4}"/>
+    <cellStyle name="Accent1 2" xfId="18" xr:uid="{2B6BACA7-E46D-4D02-9C9D-D6E19A15B706}"/>
+    <cellStyle name="Accent2 2" xfId="22" xr:uid="{CCEE17DE-7771-41D3-8D63-8D6515DF4B6B}"/>
+    <cellStyle name="Accent3 2" xfId="26" xr:uid="{58A95C4D-93C2-4011-B586-4936DB29AB69}"/>
+    <cellStyle name="Accent4 2" xfId="30" xr:uid="{DBAA8A2D-0C6F-450E-A1CD-EA3D6DC9F55A}"/>
+    <cellStyle name="Accent5 2" xfId="34" xr:uid="{AB94C307-2811-4A96-84AE-419F9D8CCD4C}"/>
+    <cellStyle name="Accent6 2" xfId="38" xr:uid="{9EB8F827-B38C-4924-A638-A2C92C37DC62}"/>
+    <cellStyle name="Bad 2" xfId="8" xr:uid="{F5AA1866-A10A-4D31-BD3D-77EC89C6E93C}"/>
+    <cellStyle name="Calculation 2" xfId="12" xr:uid="{CD0AF163-B0F9-40DD-AF6A-02F1622D9A6E}"/>
+    <cellStyle name="Check Cell 2" xfId="14" xr:uid="{10B80A0D-C9C7-405C-A7B3-0FE45C422B80}"/>
+    <cellStyle name="Explanatory Text 2" xfId="16" xr:uid="{55AB90DD-0C1B-48F2-BA30-577F821DDB0D}"/>
+    <cellStyle name="Good 2" xfId="7" xr:uid="{BE13CA0A-5665-40F8-ADD0-2A6753472189}"/>
+    <cellStyle name="Heading 1 2" xfId="3" xr:uid="{C61A378F-C151-46DF-B0C3-CA9B6B0A13DC}"/>
+    <cellStyle name="Heading 2 2" xfId="4" xr:uid="{D57A720D-E1FB-482A-A277-DD425121F9E0}"/>
+    <cellStyle name="Heading 3 2" xfId="5" xr:uid="{8E9CD3BB-68F9-4B36-8BBE-E4D5C163142B}"/>
+    <cellStyle name="Heading 4 2" xfId="6" xr:uid="{60A15386-B087-44F6-8E4D-4C38734AF757}"/>
+    <cellStyle name="Input 2" xfId="10" xr:uid="{B871F47B-ACDE-41FE-8A4B-92C29BD9C714}"/>
+    <cellStyle name="Linked Cell 2" xfId="13" xr:uid="{9A7A7A39-0496-4F2C-914A-41A1D1A1AB7F}"/>
+    <cellStyle name="Neutral 2" xfId="9" xr:uid="{DAE8BF19-034B-40A7-BBE3-565EE412BCD3}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="2" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output 2" xfId="11" xr:uid="{6257D665-4889-47CC-91D1-B40F418832DB}"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total 2" xfId="17" xr:uid="{63CA880D-7CC5-4625-9D0B-8AB0A744A082}"/>
+    <cellStyle name="Warning Text 2" xfId="15" xr:uid="{C2821A7D-145C-4B40-81DD-2D9B24196DA8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3128,19 +3668,20 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="2" max="5" width="13.77734375" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -3163,12 +3704,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="3">
-        <v>246.64142980112919</v>
+      <c r="B2" s="8">
+        <v>237</v>
       </c>
       <c r="C2" s="3">
         <v>281.92458058971829</v>
@@ -3177,21 +3718,27 @@
         <v>327.20657665901382</v>
       </c>
       <c r="E2" s="3">
-        <v>372.48895570779962</v>
+        <v>373.1213904109589</v>
       </c>
       <c r="F2" s="3">
         <v>0.60933567737192385</v>
       </c>
-      <c r="G2" s="3">
-        <v>6.142821169082116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G2" s="3" cm="1">
+        <f t="array" ref="G2:G11">TRANSPOSE(K4:T4)</f>
+        <v>5.92</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="3">
-        <v>269.01491833984801</v>
+      <c r="B3" s="8">
+        <v>272.49803277397262</v>
       </c>
       <c r="C3" s="3">
         <v>271.23977815137499</v>
@@ -3200,21 +3747,21 @@
         <v>270.97016007646812</v>
       </c>
       <c r="E3" s="3">
-        <v>270.70089073447258</v>
+        <v>269</v>
       </c>
       <c r="F3" s="3">
         <v>0.21652570658407749</v>
       </c>
       <c r="G3" s="3">
-        <v>7.3364416084441588</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="3">
-        <v>245.1866351351018</v>
+      <c r="B4" s="8">
+        <v>240</v>
       </c>
       <c r="C4" s="3">
         <v>275.415059390821</v>
@@ -3223,21 +3770,51 @@
         <v>313.11335607160959</v>
       </c>
       <c r="E4" s="3">
-        <v>350.81234395109738</v>
+        <v>350.78243150684932</v>
       </c>
       <c r="F4" s="3">
         <v>0.53784936885343004</v>
       </c>
       <c r="G4" s="3">
-        <v>5.3159288063928809</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5.09</v>
+      </c>
+      <c r="K4">
+        <v>5.92</v>
+      </c>
+      <c r="L4">
+        <v>7.2</v>
+      </c>
+      <c r="M4">
+        <v>5.09</v>
+      </c>
+      <c r="N4">
+        <v>5.6</v>
+      </c>
+      <c r="O4">
+        <v>3.93</v>
+      </c>
+      <c r="P4">
+        <v>4.29</v>
+      </c>
+      <c r="Q4">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="R4">
+        <v>4.41</v>
+      </c>
+      <c r="S4">
+        <v>6.18</v>
+      </c>
+      <c r="T4">
+        <v>6.48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="3">
-        <v>252.4169714745739</v>
+      <c r="B5" s="8">
+        <v>255.55110777397263</v>
       </c>
       <c r="C5" s="3">
         <v>250.76032404863511</v>
@@ -3246,21 +3823,21 @@
         <v>244.38833892513529</v>
       </c>
       <c r="E5" s="3">
-        <v>238.01687719209869</v>
+        <v>241.29748972602741</v>
       </c>
       <c r="F5" s="3">
         <v>0.14455686377075491</v>
       </c>
       <c r="G5" s="3">
-        <v>5.8254166973416686</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="3">
-        <v>243.09636780278751</v>
+      <c r="B6" s="8">
+        <v>238.63913893835618</v>
       </c>
       <c r="C6" s="3">
         <v>261.77057857431811</v>
@@ -3269,21 +3846,21 @@
         <v>280.53866788263389</v>
       </c>
       <c r="E6" s="3">
-        <v>299.30734564991258</v>
+        <v>299.2774383561644</v>
       </c>
       <c r="F6" s="3">
         <v>0.41112675344144239</v>
       </c>
       <c r="G6" s="3">
-        <v>4.0531224801122496</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="3">
-        <v>248.12793337443719</v>
+      <c r="B7" s="8">
+        <v>250.29343013698627</v>
       </c>
       <c r="C7" s="3">
         <v>244.6142617901933</v>
@@ -3292,21 +3869,21 @@
         <v>232.7155603605971</v>
       </c>
       <c r="E7" s="3">
-        <v>220.817584376279</v>
+        <v>223.09132876712326</v>
       </c>
       <c r="F7" s="3">
         <v>0.1374496712792137</v>
       </c>
       <c r="G7" s="3">
-        <v>4.4076541155654096</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="3">
-        <v>276.77964171906012</v>
+      <c r="B8" s="8">
+        <v>273.88444520547944</v>
       </c>
       <c r="C8" s="3">
         <v>284.01789244288511</v>
@@ -3315,21 +3892,21 @@
         <v>280.89204120564239</v>
       </c>
       <c r="E8" s="3">
-        <v>277.76633322183881</v>
+        <v>277.73642808219176</v>
       </c>
       <c r="F8" s="3">
         <v>0.35831510432466113</v>
       </c>
       <c r="G8" s="3">
-        <v>4.1872001735200177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4.1900000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="3">
-        <v>280.0278817699114</v>
+      <c r="B9" s="8">
+        <v>281.40845479452054</v>
       </c>
       <c r="C9" s="3">
         <v>272.94190845857429</v>
@@ -3338,21 +3915,21 @@
         <v>250.0178120908223</v>
       </c>
       <c r="E9" s="3">
-        <v>227.0940987025605</v>
+        <v>228.55142465753423</v>
       </c>
       <c r="F9" s="3">
         <v>0.18163255240983059</v>
       </c>
       <c r="G9" s="3">
-        <v>4.4160835164083494</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="3">
-        <v>377.6462398194185</v>
+      <c r="B10" s="8">
+        <v>359.21323972602738</v>
       </c>
       <c r="C10" s="3">
         <v>339.67870177608938</v>
@@ -3361,21 +3938,21 @@
         <v>340.11674976509971</v>
       </c>
       <c r="E10" s="3">
-        <v>342.10726366278118</v>
+        <v>342.43547945205478</v>
       </c>
       <c r="F10" s="3">
         <v>0.31044557898976338</v>
       </c>
       <c r="G10" s="3">
-        <v>6.3897199937719993</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6.18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="3">
-        <v>384.04439456882301</v>
+      <c r="B11" s="9">
+        <v>369.59616780821921</v>
       </c>
       <c r="C11" s="3">
         <v>332.73232094446502</v>
@@ -3384,13 +3961,13 @@
         <v>314.38752116477951</v>
       </c>
       <c r="E11" s="3">
-        <v>297.59539619789581</v>
+        <v>298.9611815068493</v>
       </c>
       <c r="F11" s="3">
         <v>0.1527688508933234</v>
       </c>
       <c r="G11" s="3">
-        <v>6.4834492071449201</v>
+        <v>6.48</v>
       </c>
     </row>
   </sheetData>
@@ -3402,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>